<commit_message>
teste de emprego parte 03/08/2025
</commit_message>
<xml_diff>
--- a/tk_sistema_simulaTesteEmprego/Dados.xlsx
+++ b/tk_sistema_simulaTesteEmprego/Dados.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1567,6 +1567,286 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>gggu</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>gjhh</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
+        <v>50</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Reprovado(a)</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>gggu</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>gjhh</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="M18" t="n">
+        <v>110</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Aprovado(a)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>gggu</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>gjhh</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
+        <v>190</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Aprovado(a)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ff</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>uuu</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="M20" t="n">
+        <v>60</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Aprovado(a)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>

</xml_diff>